<commit_message>
get highest row and col -> read all
</commit_message>
<xml_diff>
--- a/input/test.xlsx
+++ b/input/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">column A1</t>
   </si>
@@ -39,22 +39,70 @@
     <t xml:space="preserve">text a</t>
   </si>
   <si>
+    <t>1,23</t>
+  </si>
+  <si>
     <t xml:space="preserve">string 2</t>
   </si>
   <si>
     <t xml:space="preserve">text b</t>
   </si>
   <si>
+    <t>1,24</t>
+  </si>
+  <si>
     <t xml:space="preserve">string 3</t>
   </si>
   <si>
+    <t>1,25</t>
+  </si>
+  <si>
     <t xml:space="preserve">string 4</t>
   </si>
   <si>
+    <t>1,26</t>
+  </si>
+  <si>
     <t xml:space="preserve">string 5</t>
   </si>
   <si>
+    <t>1,27</t>
+  </si>
+  <si>
     <t xml:space="preserve">string 6</t>
+  </si>
+  <si>
+    <t>1,28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 7</t>
+  </si>
+  <si>
+    <t>1,29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 8</t>
+  </si>
+  <si>
+    <t>1,30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 9</t>
+  </si>
+  <si>
+    <t>1,31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 10</t>
+  </si>
+  <si>
+    <t>1,32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 11</t>
+  </si>
+  <si>
+    <t>1,33</t>
   </si>
 </sst>
 </file>
@@ -96,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -650,13 +699,13 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>1.23</v>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -665,15 +714,15 @@
         <v>123457</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>1.24</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -681,16 +730,16 @@
       <c r="C4">
         <v>123458</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2">
-        <v>1.2500000000000002</v>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
+      <c r="A5" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -698,16 +747,16 @@
       <c r="C5">
         <v>123459</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.2600000000000005</v>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
+      <c r="A6" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -715,16 +764,16 @@
       <c r="C6">
         <v>123460</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2">
-        <v>1.2700000000000007</v>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
+      <c r="A7" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -732,11 +781,51 @@
       <c r="C7">
         <v>123461</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.2800000000000009</v>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>